<commit_message>
QA fix bad links, errors and warnings
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -423,442 +423,644 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Additional USCDI Requirements</t>
+          <t>Is_New</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Addl_USCDI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Profile</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>FHIR Element</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>FHIR_Element</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KEEP ME HERE </t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">KEEP ME HERE </t>
+          <t>Contact Detail</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">KEEP ME HERE </t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Patient.telecom</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Contact Detail</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[US Core Patient Profile]</t>
+          <t>A Communication Language</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Patient.telecom</t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Patient.communication</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A Communication Language</t>
+          <t>True</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[US Core Patient Profile]</t>
+          <t>An Interpreter Required Flag</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Patient.communication</t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Patient.extension:interpreterRequired</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>An Interpreter Required Flag</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Encounter.extension:interpreterRequired</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>A Race</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Patient.extension:race</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
         <is>
           <t>An Ethnicity</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Patient.extension:ethnicity</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
         <is>
           <t>A Tribal Affiliation</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>Patient.extension:tribalAffiliation</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
         <is>
           <t>A Sex</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>Patient.extension:sex</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Gender Identity</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Patient.extension:genderIdentity</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Date Of Death</t>
+          <t>True</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[US Core Patient Profile]</t>
+          <t>Sex Parameter For Clinical Use</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Patient.extension:sexParameterForClinicalUse</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Previous Address</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[US Core Patient Profile]</t>
+          <t>Gender Identity</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Patient.address.use or Patient.address.period</t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Patient.extension:genderIdentity</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>True</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[US Core Patient Profile]</t>
+          <t>Personal Pronouns</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Patient.name.use or Patient.name.period</t>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Patient.extension:personalPronouns</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Date Of Death</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Patient.deceased[x]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Address Use</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Patient.address.use</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Address Period</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Patient.address.period</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Name Use</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Patient.name.use</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Name Period</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Patient.name.period</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Suffix</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>[US Core Patient Profile]</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>Patient.name.suffix</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
         <is>
           <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>[US Core ServiceRequest Profile]</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
         <is>
           <t>ServiceRequest.reasonCode</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
         <is>
           <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>[US Core ServiceRequest Profile]</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>ServiceRequest.reasonReference</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>A Reason Or Indication For Referral Or Consultation</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>[US Core Procedure Profile]</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Procedure.reasonCode</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>A Reason Or Indication For Referral Or Consultation</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>[US Core Procedure Profile]</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Procedure.reasonReference</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>The Reason Or Indication For The Prescription</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>[US Core MedicationRequest Profile]</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>MedicationRequest.reasonCode</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>The Reason Or Indication For The Prescription</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>[US Core MedicationRequest Profile]</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MedicationRequest.reasonReference</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Medication Adherence</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>[US Core MedicationRequest Profile]</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MedicationRequest.extension:medicationAdherence</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>A Reference To The Request For The Procedure</t>
+          <t>True</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[US Core Procedure Profile]</t>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Procedure.basedOn</t>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Procedure.performer</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Procedure.performer.actor</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Procedure.reasonCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Procedure.reasonReference</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>The Reason Or Indication For The Prescription</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>MedicationRequest.reasonCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>The Reason Or Indication For The Prescription</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>MedicationRequest.reasonReference</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Medication Adherence</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>MedicationRequest.extension:medicationAdherence</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>A Reference To The Request For The Procedure</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Procedure.basedOn</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>US Core Document Category</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>[US Core DocumentReference Profile]</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>US Core DocumentReference Profile</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
         <is>
           <t>DocumentReference.category:uscore</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
         <is>
           <t>References To An Associated Survey, Assessment, Or Screening Tool</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>[US Core Simple Observation Profile]</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>Observation.derivedFrom</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
         <is>
           <t>Specimen Source Site</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>[US Core Specimen Profile]</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>Specimen.collection</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Specimen Source Site</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>[US Core Specimen Profile]</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>Specimen.collection.bodySite</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Specimen Condition Acceptability</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>[US Core Specimen Profile]</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>Specimen.condition</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Health Status Assessments</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Observation.category:us-core</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update ignorewarnings annotations, tables for download
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -441,6 +441,11 @@
           <t>FHIR_Element</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>combo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -459,6 +464,11 @@
           <t>Patient.telecom</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.telecom</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -477,6 +487,11 @@
           <t>Patient.communication</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.communication</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -486,7 +501,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>An Interpreter Required Flag</t>
+          <t>An Interpreter Needed Flag</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -497,6 +512,11 @@
       <c r="D4" t="inlineStr">
         <is>
           <t>Patient.extension:interpreterRequired</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:interpreterRequired</t>
         </is>
       </c>
     </row>
@@ -508,7 +528,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>An Interpreter Required Flag</t>
+          <t>An Interpreter Needed Flag</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -519,6 +539,11 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>Encounter.extension:interpreterRequired</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>US Core Encounter Profile-Encounter.extension:interpreterRequired</t>
         </is>
       </c>
     </row>
@@ -539,6 +564,11 @@
           <t>Patient.extension:race</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:race</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -557,6 +587,11 @@
           <t>Patient.extension:ethnicity</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:ethnicity</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -575,6 +610,11 @@
           <t>Patient.extension:tribalAffiliation</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:tribalAffiliation</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -593,6 +633,11 @@
           <t>Patient.extension:sex</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:sex</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -613,6 +658,11 @@
       <c r="D10" t="inlineStr">
         <is>
           <t>Patient.extension:sexParameterForClinicalUse</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:sexParameterForClinicalUse</t>
         </is>
       </c>
     </row>
@@ -633,6 +683,11 @@
           <t>Patient.extension:genderIdentity</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:genderIdentity</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -653,6 +708,11 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>Patient.extension:personalPronouns</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.extension:personalPronouns</t>
         </is>
       </c>
     </row>
@@ -673,6 +733,11 @@
           <t>Patient.deceased[x]</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.deceased[x]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -691,6 +756,11 @@
           <t>Patient.address.use</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.address.use</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -709,6 +779,11 @@
           <t>Patient.address.period</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.address.period</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -727,6 +802,11 @@
           <t>Patient.name.use</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.name.use</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -745,6 +825,11 @@
           <t>Patient.name.period</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.name.period</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -763,6 +848,11 @@
           <t>Patient.name.suffix</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>US Core Patient Profile-Patient.name.suffix</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -781,6 +871,11 @@
           <t>ServiceRequest.reasonCode</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile-ServiceRequest.reasonCode</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -799,6 +894,11 @@
           <t>ServiceRequest.reasonReference</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>US Core ServiceRequest Profile-ServiceRequest.reasonReference</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -821,6 +921,11 @@
           <t>Procedure.performer</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile-Procedure.performer</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -841,6 +946,11 @@
       <c r="D22" t="inlineStr">
         <is>
           <t>Procedure.performer.actor</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile-Procedure.performer.actor</t>
         </is>
       </c>
     </row>
@@ -861,6 +971,11 @@
           <t>Procedure.reasonCode</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile-Procedure.reasonCode</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -879,6 +994,11 @@
           <t>Procedure.reasonReference</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile-Procedure.reasonReference</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -897,6 +1017,11 @@
           <t>MedicationRequest.reasonCode</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile-MedicationRequest.reasonCode</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -915,6 +1040,11 @@
           <t>MedicationRequest.reasonReference</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile-MedicationRequest.reasonReference</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -933,6 +1063,11 @@
           <t>MedicationRequest.extension:medicationAdherence</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>US Core MedicationRequest Profile-MedicationRequest.extension:medicationAdherence</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -951,6 +1086,11 @@
           <t>Procedure.basedOn</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>US Core Procedure Profile-Procedure.basedOn</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -969,6 +1109,11 @@
           <t>DocumentReference.category:uscore</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>US Core DocumentReference Profile-DocumentReference.category:uscore</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -987,6 +1132,11 @@
           <t>Observation.derivedFrom</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile-Observation.derivedFrom</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -1005,6 +1155,11 @@
           <t>Specimen.collection</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile-Specimen.collection</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -1023,6 +1178,11 @@
           <t>Specimen.collection.bodySite</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile-Specimen.collection.bodySite</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -1041,6 +1201,11 @@
           <t>Specimen.condition</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>US Core Specimen Profile-Specimen.condition</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1061,6 +1226,92 @@
       <c r="D34" t="inlineStr">
         <is>
           <t>Observation.category:us-core</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>US Core Simple Observation Profile-Observation.category:us-core</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Pregnancy Status</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>US Core Observation Pregnancy Intent Profile</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Observation.performer</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>US Core Observation Pregnancy Intent Profile-Observation.performer</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Sexual Orientation</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>US Core Observation Sexual Orientation Profile</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Observation.performer</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>US Core Observation Sexual Orientation Profile-Observation.performer</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Pregnancy Status</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>US Core Observation Pregnancy Status Profile</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Observation.performer</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>US Core Observation Pregnancy Status Profile-Observation.performer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update to latest publisher and address new QA warnings and errors. update terminology tables update csv and excel files
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -1219,11 +1219,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
           <t>Health Status Assessments</t>
@@ -1246,11 +1242,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
           <t>Health Status Assessments</t>
@@ -1346,11 +1338,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1373,11 +1361,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1400,11 +1384,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1427,11 +1407,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1454,11 +1430,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1481,11 +1453,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1508,11 +1476,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
           <t>Provenance Author</t>
@@ -1535,11 +1499,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
           <t>Orders</t>
@@ -1562,11 +1522,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
           <t>Laboratory Tests</t>

</xml_diff>

<commit_message>
QA minor copy edits
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="additional-uscdi-requirements.csv" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="additional-uscdi-requirements.csv" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1545,6 +1545,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Excel and CVS to the images/table folde
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="additional-uscdi-requirements.csv" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="additional-uscdi-requirements.csv" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1544,7 +1544,223 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Care Plan</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>US Core CarePlan Profile</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>CarePlan.addresses</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>US Core CarePlan Profile-CarePlan.addresses</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Family Health History</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>US Core FamilyMemberHistory Profile</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>FamilyMemberHistory.extension:recorder</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>US Core FamilyMemberHistory Profile-FamilyMemberHistory.extension:recorder</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Device.udiCarrier</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.udiCarrier</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Device.distinctIdentifier</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.distinctIdentifier</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Device.manufactureDate</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.manufactureDate</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Device.expirationDate</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.expirationDate</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Device.lotNumber</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.lotNumber</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Unique Device Identifier</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>US Core Device Profile</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Device.serialNumber</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>US Core Device Profile-Device.serialNumber</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove PMO servicerequest profile FHIR-55597 partially applied
</commit_message>
<xml_diff>
--- a/input/images/tables/additional-uscdi-requirements.xlsx
+++ b/input/images/tables/additional-uscdi-requirements.xlsx
@@ -632,14 +632,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sex Parameter For Clinical Use</t>
+          <t>Date Of Death</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -649,24 +645,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Patient.extension:sexParameterForClinicalUse</t>
+          <t>Patient.deceased[x]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.extension:sexParameterForClinicalUse</t>
+          <t>US Core Patient Profile-Patient.deceased[x]</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gender Identity</t>
+          <t>Address Use</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -676,24 +668,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Patient.extension:genderIdentity</t>
+          <t>Patient.address.use</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.extension:genderIdentity</t>
+          <t>US Core Patient Profile-Patient.address.use</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Personal Pronouns</t>
+          <t>Address Period</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -703,12 +691,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Patient.extension:personalPronouns</t>
+          <t>Patient.address.period</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.extension:personalPronouns</t>
+          <t>US Core Patient Profile-Patient.address.period</t>
         </is>
       </c>
     </row>
@@ -716,7 +704,7 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Date Of Death</t>
+          <t>Previous Name</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -726,12 +714,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Patient.deceased[x]</t>
+          <t>Patient.name.use</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.deceased[x]</t>
+          <t>US Core Patient Profile-Patient.name.use</t>
         </is>
       </c>
     </row>
@@ -739,7 +727,7 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Address Use</t>
+          <t>Name Period</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -749,12 +737,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Patient.address.use</t>
+          <t>Patient.name.period</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.address.use</t>
+          <t>US Core Patient Profile-Patient.name.period</t>
         </is>
       </c>
     </row>
@@ -762,7 +750,7 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Address Period</t>
+          <t>Suffix</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -772,12 +760,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Patient.address.period</t>
+          <t>Patient.name.suffix</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.address.period</t>
+          <t>US Core Patient Profile-Patient.name.suffix</t>
         </is>
       </c>
     </row>
@@ -785,22 +773,22 @@
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Previous Name</t>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Patient.name.use</t>
+          <t>ServiceRequest.reasonCode</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.name.use</t>
+          <t>US Core ServiceRequest Profile-ServiceRequest.reasonCode</t>
         </is>
       </c>
     </row>
@@ -808,22 +796,22 @@
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Name Period</t>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Patient.name.period</t>
+          <t>ServiceRequest.reasonReference</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.name.period</t>
+          <t>US Core ServiceRequest Profile-ServiceRequest.reasonReference</t>
         </is>
       </c>
     </row>
@@ -831,22 +819,22 @@
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Suffix</t>
+          <t>A Reason Or Indication For Referral Or Consultation</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>US Core Patient Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Patient.name.suffix</t>
+          <t>Procedure.performer</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>US Core Patient Profile-Patient.name.suffix</t>
+          <t>US Core Procedure Profile-Procedure.performer</t>
         </is>
       </c>
     </row>
@@ -859,17 +847,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonCode</t>
+          <t>Procedure.performer.actor</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile-ServiceRequest.reasonCode</t>
+          <t>US Core Procedure Profile-Procedure.performer.actor</t>
         </is>
       </c>
     </row>
@@ -882,17 +870,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>ServiceRequest.reasonReference</t>
+          <t>Procedure.reasonCode</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile-ServiceRequest.reasonReference</t>
+          <t>US Core Procedure Profile-Procedure.reasonCode</t>
         </is>
       </c>
     </row>
@@ -910,12 +898,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Procedure.performer</t>
+          <t>Procedure.reasonReference</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile-Procedure.performer</t>
+          <t>US Core Procedure Profile-Procedure.reasonReference</t>
         </is>
       </c>
     </row>
@@ -923,22 +911,22 @@
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A Reason Or Indication For Referral Or Consultation</t>
+          <t>The Reason Or Indication For The Prescription</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Procedure.performer.actor</t>
+          <t>MedicationRequest.reasonCode</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile-Procedure.performer.actor</t>
+          <t>US Core MedicationRequest Profile-MedicationRequest.reasonCode</t>
         </is>
       </c>
     </row>
@@ -946,22 +934,22 @@
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A Reason Or Indication For Referral Or Consultation</t>
+          <t>The Reason Or Indication For The Prescription</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Procedure.reasonCode</t>
+          <t>MedicationRequest.reasonReference</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile-Procedure.reasonCode</t>
+          <t>US Core MedicationRequest Profile-MedicationRequest.reasonReference</t>
         </is>
       </c>
     </row>
@@ -969,22 +957,22 @@
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A Reason Or Indication For Referral Or Consultation</t>
+          <t>Medication Adherence</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core MedicationRequest Profile</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Procedure.reasonReference</t>
+          <t>MedicationRequest.extension:medicationAdherence</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile-Procedure.reasonReference</t>
+          <t>US Core MedicationRequest Profile-MedicationRequest.extension:medicationAdherence</t>
         </is>
       </c>
     </row>
@@ -992,22 +980,22 @@
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>The Reason Or Indication For The Prescription</t>
+          <t>A Reference To The Request For The Procedure</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Procedure Profile</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MedicationRequest.reasonCode</t>
+          <t>Procedure.basedOn</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile-MedicationRequest.reasonCode</t>
+          <t>US Core Procedure Profile-Procedure.basedOn</t>
         </is>
       </c>
     </row>
@@ -1015,22 +1003,22 @@
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The Reason Or Indication For The Prescription</t>
+          <t>US Core Document Category</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core DocumentReference Profile</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MedicationRequest.reasonReference</t>
+          <t>DocumentReference.category:uscore</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile-MedicationRequest.reasonReference</t>
+          <t>US Core DocumentReference Profile-DocumentReference.category:uscore</t>
         </is>
       </c>
     </row>
@@ -1038,22 +1026,22 @@
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Medication Adherence</t>
+          <t>References To An Associated Survey, Assessment, Or Screening Tool</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile</t>
+          <t>US Core Simple Observation Profile</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MedicationRequest.extension:medicationAdherence</t>
+          <t>Observation.derivedFrom</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>US Core MedicationRequest Profile-MedicationRequest.extension:medicationAdherence</t>
+          <t>US Core Simple Observation Profile-Observation.derivedFrom</t>
         </is>
       </c>
     </row>
@@ -1061,22 +1049,22 @@
       <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A Reference To The Request For The Procedure</t>
+          <t>Specimen Source Site</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Procedure.basedOn</t>
+          <t>Specimen.collection</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>US Core Procedure Profile-Procedure.basedOn</t>
+          <t>US Core Specimen Profile-Specimen.collection</t>
         </is>
       </c>
     </row>
@@ -1084,22 +1072,22 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>US Core Document Category</t>
+          <t>Specimen Source Site</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>DocumentReference.category:uscore</t>
+          <t>Specimen.collection.bodySite</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>US Core DocumentReference Profile-DocumentReference.category:uscore</t>
+          <t>US Core Specimen Profile-Specimen.collection.bodySite</t>
         </is>
       </c>
     </row>
@@ -1107,22 +1095,22 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>References To An Associated Survey, Assessment, Or Screening Tool</t>
+          <t>Specimen Condition Acceptability</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile</t>
+          <t>US Core Specimen Profile</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Observation.derivedFrom</t>
+          <t>Specimen.condition</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile-Observation.derivedFrom</t>
+          <t>US Core Specimen Profile-Specimen.condition</t>
         </is>
       </c>
     </row>
@@ -1130,22 +1118,22 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Specimen Source Site</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Simple Observation Profile</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Specimen.collection</t>
+          <t>Observation.category:us-core</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile-Specimen.collection</t>
+          <t>US Core Simple Observation Profile-Observation.category:us-core</t>
         </is>
       </c>
     </row>
@@ -1153,22 +1141,22 @@
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Specimen Source Site</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Observation Screening Assessment Profile</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Specimen.collection.bodySite</t>
+          <t>Observation.category:screening-assessment</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile-Specimen.collection.bodySite</t>
+          <t>US Core Observation Screening Assessment Profile-Observation.category:screening-assessment</t>
         </is>
       </c>
     </row>
@@ -1176,22 +1164,22 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Specimen Condition Acceptability</t>
+          <t>Health Status Assessments</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Specimen.condition</t>
+          <t>Condition.category:screening-assessment</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>US Core Specimen Profile-Specimen.condition</t>
+          <t>US Core Condition Problems and Health Concerns Profile-Condition.category:screening-assessment</t>
         </is>
       </c>
     </row>
@@ -1199,22 +1187,22 @@
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Health Status Assessments</t>
+          <t>Pregnancy Status</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile</t>
+          <t>US Core Observation Pregnancy Intent Profile</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Observation.category:us-core</t>
+          <t>Observation.performer</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>US Core Simple Observation Profile-Observation.category:us-core</t>
+          <t>US Core Observation Pregnancy Intent Profile-Observation.performer</t>
         </is>
       </c>
     </row>
@@ -1222,22 +1210,22 @@
       <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Health Status Assessments</t>
+          <t>Pregnancy Status</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile</t>
+          <t>US Core Observation Pregnancy Status Profile</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Observation.category:screening-assessment</t>
+          <t>Observation.performer</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>US Core Observation Screening Assessment Profile-Observation.category:screening-assessment</t>
+          <t>US Core Observation Pregnancy Status Profile-Observation.performer</t>
         </is>
       </c>
     </row>
@@ -1245,22 +1233,22 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Health Status Assessments</t>
+          <t>Provenance Author</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core AllergyIntolerance Profile</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Condition.category:screening-assessment</t>
+          <t>AllergyIntolerance.recorder</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile-Condition.category:screening-assessment</t>
+          <t>US Core AllergyIntolerance Profile-AllergyIntolerance.recorder</t>
         </is>
       </c>
     </row>
@@ -1268,12 +1256,12 @@
       <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Pregnancy Status</t>
+          <t>Provenance Author</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Intent Profile</t>
+          <t>US Core Care Experience Preference Profile</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1283,34 +1271,30 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Intent Profile-Observation.performer</t>
+          <t>US Core Care Experience Preference Profile-Observation.performer</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>!</t>
-        </is>
-      </c>
+      <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sexual Orientation</t>
+          <t>Provenance Author</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile</t>
+          <t>US Core CarePlan Profile</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Observation.performer</t>
+          <t>CarePlan.contributor</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>US Core Observation Sexual Orientation Profile-Observation.performer</t>
+          <t>US Core CarePlan Profile-CarePlan.contributor</t>
         </is>
       </c>
     </row>
@@ -1318,22 +1302,22 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Pregnancy Status</t>
+          <t>Provenance Author</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile</t>
+          <t>US Core Condition Encounter Diagnosis Profile</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Observation.performer</t>
+          <t>Condition.recorder</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>US Core Observation Pregnancy Status Profile-Observation.performer</t>
+          <t>US Core Condition Encounter Diagnosis Profile-Condition.recorder</t>
         </is>
       </c>
     </row>
@@ -1346,17 +1330,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>US Core AllergyIntolerance Profile</t>
+          <t>US Core Condition Problems and Health Concerns Profile</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>AllergyIntolerance.recorder</t>
+          <t>Condition.recorder</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>US Core AllergyIntolerance Profile-AllergyIntolerance.recorder</t>
+          <t>US Core Condition Problems and Health Concerns Profile-Condition.recorder</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1353,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>US Core Care Experience Preference Profile</t>
+          <t>US Core Observation Occupation Profile</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1379,7 +1363,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>US Core Care Experience Preference Profile-Observation.performer</t>
+          <t>US Core Observation Occupation Profile-Observation.performer</t>
         </is>
       </c>
     </row>
@@ -1392,17 +1376,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile</t>
+          <t>US Core Treatment Intervention Preference Profile</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>CarePlan.contributor</t>
+          <t>Observation.performer</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile-CarePlan.contributor</t>
+          <t>US Core Treatment Intervention Preference Profile-Observation.performer</t>
         </is>
       </c>
     </row>
@@ -1410,22 +1394,22 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Provenance Author</t>
+          <t>Orders</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile</t>
+          <t>US Core ServiceRequest Profile</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Condition.recorder</t>
+          <t>ServiceRequest.code.text</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>US Core Condition Encounter Diagnosis Profile-Condition.recorder</t>
+          <t>US Core ServiceRequest Profile-ServiceRequest.code.text</t>
         </is>
       </c>
     </row>
@@ -1433,22 +1417,22 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Provenance Author</t>
+          <t>Laboratory Tests</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile</t>
+          <t>US Core Laboratory Result Observation Profile</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Condition.recorder</t>
+          <t>Observation.code.text</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>US Core Condition Problems and Health Concerns Profile-Condition.recorder</t>
+          <t>US Core Laboratory Result Observation Profile-Observation.code.text</t>
         </is>
       </c>
     </row>
@@ -1456,22 +1440,22 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Provenance Author</t>
+          <t>Care Plan</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile</t>
+          <t>US Core CarePlan Profile</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Observation.performer</t>
+          <t>CarePlan.addresses</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>US Core Observation Occupation Profile-Observation.performer</t>
+          <t>US Core CarePlan Profile-CarePlan.addresses</t>
         </is>
       </c>
     </row>
@@ -1479,22 +1463,22 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Provenance Author</t>
+          <t>Family Health History</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>US Core Treatment Intervention Preference Profile</t>
+          <t>US Core FamilyMemberHistory Profile</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Observation.performer</t>
+          <t>FamilyMemberHistory.extension:recorder</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>US Core Treatment Intervention Preference Profile-Observation.performer</t>
+          <t>US Core FamilyMemberHistory Profile-FamilyMemberHistory.extension:recorder</t>
         </is>
       </c>
     </row>
@@ -1502,22 +1486,22 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Orders</t>
+          <t>Unique Device Identifier</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile</t>
+          <t>US Core Device Profile</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ServiceRequest.code.text</t>
+          <t>Device.udiCarrier</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>US Core ServiceRequest Profile-ServiceRequest.code.text</t>
+          <t>US Core Device Profile-Device.udiCarrier</t>
         </is>
       </c>
     </row>
@@ -1525,85 +1509,73 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Laboratory Tests</t>
+          <t>Unique Device Identifier</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile</t>
+          <t>US Core Device Profile</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Observation.code.text</t>
+          <t>Device.distinctIdentifier</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>US Core Laboratory Result Observation Profile-Observation.code.text</t>
+          <t>US Core Device Profile-Device.distinctIdentifier</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Care Plan</t>
+          <t>Unique Device Identifier</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile</t>
+          <t>US Core Device Profile</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>CarePlan.addresses</t>
+          <t>Device.manufactureDate</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>US Core CarePlan Profile-CarePlan.addresses</t>
+          <t>US Core Device Profile-Device.manufactureDate</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Family Health History</t>
+          <t>Unique Device Identifier</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>US Core FamilyMemberHistory Profile</t>
+          <t>US Core Device Profile</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>FamilyMemberHistory.extension:recorder</t>
+          <t>Device.expirationDate</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>US Core FamilyMemberHistory Profile-FamilyMemberHistory.extension:recorder</t>
+          <t>US Core Device Profile-Device.expirationDate</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
           <t>Unique Device Identifier</t>
@@ -1616,21 +1588,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Device.udiCarrier</t>
+          <t>Device.lotNumber</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>US Core Device Profile-Device.udiCarrier</t>
+          <t>US Core Device Profile-Device.lotNumber</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+      <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
           <t>Unique Device Identifier</t>
@@ -1643,118 +1611,10 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Device.distinctIdentifier</t>
+          <t>Device.serialNumber</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
-        <is>
-          <t>US Core Device Profile-Device.distinctIdentifier</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>US Core Device Profile</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Device.manufactureDate</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>US Core Device Profile-Device.manufactureDate</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>US Core Device Profile</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Device.expirationDate</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>US Core Device Profile-Device.expirationDate</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>US Core Device Profile</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Device.lotNumber</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>US Core Device Profile-Device.lotNumber</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Unique Device Identifier</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>US Core Device Profile</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Device.serialNumber</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
         <is>
           <t>US Core Device Profile-Device.serialNumber</t>
         </is>

</xml_diff>